<commit_message>
minor updates to the test class and final test cases
minor updates to the test class and final test cases
</commit_message>
<xml_diff>
--- a/docs/TestCases.xlsx
+++ b/docs/TestCases.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="176" documentId="8_{768CC40A-DB5A-4F52-B807-16F076D631BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B1A7599-3E6C-4F48-81E8-FA2F6FE29B6D}"/>
+  <xr:revisionPtr revIDLastSave="349" documentId="8_{768CC40A-DB5A-4F52-B807-16F076D631BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24EEFAF1-0528-4252-A524-CDA98ACC53A4}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5595" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Screenshots" sheetId="3" r:id="rId2"/>
-    <sheet name="Todos" sheetId="4" r:id="rId3"/>
+    <sheet name="LoginPage Observations" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$2:$P$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$2:$Q$3</definedName>
     <definedName name="ColumnTitle1">Guests[[#Headers],[Test Case ID]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">TestCases!$2:$2</definedName>
   </definedNames>
@@ -22,7 +22,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
   <si>
     <t>NOTES</t>
   </si>
   <si>
-    <t>LoginTest Cases</t>
-  </si>
-  <si>
     <t>Test Case ID</t>
   </si>
   <si>
@@ -47,36 +49,21 @@
     <t>Steps</t>
   </si>
   <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
     <t>User successfully logs in with valid credentials</t>
   </si>
   <si>
     <t>LoginTC1</t>
   </si>
   <si>
-    <t>after incomplete attempt, entering the correect credenitals will allow you to login</t>
-  </si>
-  <si>
-    <t>MFA Screen should be presented to user</t>
-  </si>
-  <si>
     <t>LoginTC2</t>
   </si>
   <si>
     <t>User successfully logs in with invalid credentials</t>
   </si>
   <si>
-    <t>Invalid login scrren</t>
-  </si>
-  <si>
     <t>Multi-Factor Authentication Page</t>
   </si>
   <si>
-    <t>Error Message should be presented to user</t>
-  </si>
-  <si>
     <t>User clicks on the "Do not have an account?" link</t>
   </si>
   <si>
@@ -87,15 +74,6 @@
   </si>
   <si>
     <t>Cross-browser testing</t>
-  </si>
-  <si>
-    <t>Red Alert box is shown</t>
-  </si>
-  <si>
-    <t>Sign-in Button without any entriess</t>
-  </si>
-  <si>
-    <t>after incomplete attempt, entering the correct credenitals will allow you to login</t>
   </si>
   <si>
     <t>Load Testing</t>
@@ -111,12 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">  Given the user is on the login page
-  When the user enters a valid Email and Password
-  And clicks the Sign-in button
-  Then the user should be directed  to the Multi-Factor Authentication Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Given the user is on the login page
   When the user enters an invalid Email and Password
   And clicks the Sign-in button
   Then the user will receive error message "Invalid username/password. Please contact your system administrator for assistance."</t>
@@ -127,88 +99,231 @@
   Then the user will be presented with the Verify Identity Screen</t>
   </si>
   <si>
+    <t>Don'tHaveAnAccount Registration Screen</t>
+  </si>
+  <si>
+    <t>Forgot Password Verify Identity Screen</t>
+  </si>
+  <si>
+    <t>Login Page Link</t>
+  </si>
+  <si>
+    <t>NinjaOne</t>
+  </si>
+  <si>
+    <t>"Keep me signed in" checkbox on</t>
+  </si>
+  <si>
+    <t>"Keep me signed in" checkbox off</t>
+  </si>
+  <si>
+    <t>Error popup doesn't always show</t>
+  </si>
+  <si>
+    <t>Error message for invalid login is different when one field is not present vs. when both fields are present vs. when neither field values are present</t>
+  </si>
+  <si>
+    <t>Error message says, "username", but the field's label is "Email"</t>
+  </si>
+  <si>
+    <t>SQL Injection to input fields</t>
+  </si>
+  <si>
+    <t>Max out Email and password input values</t>
+  </si>
+  <si>
+    <t>run Axe Report and check for Accessibility violations</t>
+  </si>
+  <si>
     <t xml:space="preserve">  Given the user is on the login page
-  When the user  clicks on the "Do not have an account?" link 
+  When the user clicks on the "Do not have an account?" link 
   Then the user will be presented with the Registration Screen</t>
   </si>
   <si>
-    <t>Don'tHaveAnAccount Registration Screen</t>
-  </si>
-  <si>
-    <t>Forgot Password Verify Identity Screen</t>
-  </si>
-  <si>
-    <t>Login Page Link</t>
-  </si>
-  <si>
-    <t>NinjaOne</t>
+    <t>Screenshots Worksheet Link</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user is on the login page
+  When the user enters a valid Email and Password
+  And clicks the Sign-in button
+  Then the user should be directed to the Multi-Factor Authentication Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user is on the login page using different browsers
+  When the test cases are run 
+  Then similar behavior/results should be presented across browsers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user is on the login page and received error message for invalid login
+  When the user enters a valid Email and Password
+  And clicks the Sign-in button
+  Then the user should be directed to the Multi-Factor Authentication Page</t>
+  </si>
+  <si>
+    <t>The login page should adhere to accessibility guidelines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user has NOT checked the "Keep me signed in" checkbox and logs in
+  When the user closes the browser and revisits the login page  
+  Then the user should NOT be automatically signed in and presented with the home page</t>
+  </si>
+  <si>
+    <t>LoginTC3</t>
+  </si>
+  <si>
+    <t>LoginTC4</t>
+  </si>
+  <si>
+    <t>LoginTC5</t>
+  </si>
+  <si>
+    <t>LoginTC6</t>
+  </si>
+  <si>
+    <t>LoginTC7</t>
+  </si>
+  <si>
+    <t>LoginTC8</t>
+  </si>
+  <si>
+    <t>LoginTC9</t>
+  </si>
+  <si>
+    <t>LoginTC10</t>
+  </si>
+  <si>
+    <t>LoginTC11</t>
+  </si>
+  <si>
+    <t>LoginTC12</t>
+  </si>
+  <si>
+    <t>LoginTC13</t>
+  </si>
+  <si>
+    <t>LoginTC14</t>
+  </si>
+  <si>
+    <t>LoginTC15</t>
+  </si>
+  <si>
+    <t>LoginTC16</t>
+  </si>
+  <si>
+    <t>LoginTC17</t>
+  </si>
+  <si>
+    <t>LoginTC18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user is on the login page
+  When the user enters a valid Email using ALL CAPS or Mixed CAPS and a valid Password
+  And clicks the Sign-in button
+  Then the user should be directed to the Multi-Factor Authentication Page</t>
+  </si>
+  <si>
+    <t>Email field is case insensitive</t>
+  </si>
+  <si>
+    <t>Password field is case sensitive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user is on the login page
+  When the user enters a valid Email using ALL CAPS or Mixed CAPS and a valid Password with ALL CAPS or Mixed CAPS
+  And clicks the Sign-in button
+  Then the user will receive error message "Invalid username/password. Please contact your system administrator for assistance."</t>
+  </si>
+  <si>
+    <t>Test how the login functionality works are multiple concurrent users are introduced.</t>
   </si>
   <si>
     <t xml:space="preserve">  Given the user is on the login page
   When the user  presses the Tab button multiple times 
-  Then the user will be able to enter the Email and Password fields and login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Given the user is on the login page using different browsers
-  When the test cases are run 
-  Then similar results should be received</t>
-  </si>
-  <si>
-    <t>"Keep me signed in" checkbox on</t>
-  </si>
-  <si>
-    <t>"Keep me signed in" checkbox off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password is visible when "Eye" </t>
-  </si>
-  <si>
-    <t>Looks like there is a bug, that the Eye button is not presented when clicking away and then reenter</t>
-  </si>
-  <si>
-    <t>Forein Characters</t>
-  </si>
-  <si>
-    <t>Spell Check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Videos </t>
-  </si>
-  <si>
-    <t>Issues Found:</t>
-  </si>
-  <si>
-    <t>Error popup doesn't always show</t>
-  </si>
-  <si>
-    <t>Here the popup shows, but the invalid text message doesn't who in the main dialog box</t>
-  </si>
-  <si>
-    <t>below, the red pop up doesn't show, but error message for invalid username/password is shown in the main dialog area</t>
-  </si>
-  <si>
-    <t>Email field is case insensitive whle password field should be case sensitive</t>
-  </si>
-  <si>
-    <t>Error message for invalid login is different when one field is not present vs. when both fields are present vs. when neither field values are present</t>
-  </si>
-  <si>
-    <t>Looks like the login &amp; password fields can taken more values than really needed for an email or password</t>
-  </si>
-  <si>
-    <t>Todos:</t>
-  </si>
-  <si>
-    <t>Error message says, "username", but the field's label is "Email"</t>
-  </si>
-  <si>
-    <t>SQL Injection to input fields</t>
-  </si>
-  <si>
-    <t>Max out Email and password input values</t>
-  </si>
-  <si>
-    <t>run Axe Report and check for Accessibility violations</t>
+  Then the user will be able to move to and enter values into the Email and Password fields and login successfully</t>
+  </si>
+  <si>
+    <t>Automated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user is on the login page
+  When the user enters SQL injection strings into Email and Password fields
+  And clicks the Sign-in button 
+  Then the user will receive error message "Invalid username/password. Please contact your system administrator for assistance."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user is on the login page
+  When the user enters more than 100 characters into Email and Password fields 
+  And clicks the Sign-in button
+  Then the user will receive error message "Invalid username/password. Please contact your system administrator for assistance."</t>
+  </si>
+  <si>
+    <t>after incomplete attempt, entering the correct credentials will allow you to login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user has checked the "Keep me signed in" checkbox and logs in
+  When the user closes the browser and revisits the login page  
+  Then the user should be automatically signed in and presented with the Get Started page</t>
+  </si>
+  <si>
+    <t>Login Test Cases</t>
+  </si>
+  <si>
+    <t>Password Visibility is turned on</t>
+  </si>
+  <si>
+    <t>Password Visibility is turned on then off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given the user is on the login page and enters values into the Password text box
+  When the user clicks on the Password Visibility Toggle
+  Then the values of the Password text box should be visible to the user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Given that the user has turned on the Password Visibility Toggle
+  When the user turns off the Password Visibility Toggle
+  Then the values of the Password text box should NOT be visible to the user</t>
+  </si>
+  <si>
+    <t>Sign-in Button without any entries</t>
+  </si>
+  <si>
+    <t>Foreign Characters</t>
+  </si>
+  <si>
+    <t>Invalid login screen</t>
+  </si>
+  <si>
+    <t>Minor Issues/Observations</t>
+  </si>
+  <si>
+    <t>Looks like the login &amp; password fields can taken more values than really needed for an email or password; consider putting a limit on these fields</t>
+  </si>
+  <si>
+    <t>the Password Visibility Toggle button is not presented when clicking away from the password field and clicking back into the password field; The only way to get it back is to clear the field and re-enter.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Here the error popup shows, but the invalid text message is not displayed in the main dialog box</t>
+  </si>
+  <si>
+    <t>below, the error popup doesn't show, but error message for invalid username/password is shown in the main dialog area</t>
   </si>
 </sst>
 </file>
@@ -221,7 +336,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Trebuchet MS"/>
@@ -269,8 +384,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +402,18 @@
       <patternFill patternType="lightVertical">
         <fgColor indexed="46"/>
         <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -333,7 +466,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -345,14 +478,23 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -801,16 +943,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>215377</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>174476</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>211567</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>170666</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -845,16 +987,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>49530</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>150597</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>58304</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209652</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>54494</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -877,8 +1019,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="12992100"/>
-          <a:ext cx="14384757" cy="8268854"/>
+          <a:off x="659130" y="10146030"/>
+          <a:ext cx="14371422" cy="8190749"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3448348</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>133598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D238C20C-09AB-3556-834C-AD9FA0919635}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="22677120"/>
+          <a:ext cx="3436918" cy="2865368"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -890,15 +1076,20 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Guests" displayName="Guests" ref="A2:E20" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A2:E20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Guests" displayName="Guests" ref="A2:F20" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A2:F20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataCellStyle="Date"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Scenario" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Steps" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{DA760A76-A5E1-412A-871D-7B1F42D497AC}" name="Expected Result"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="NOTES" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{B466EF75-CE13-44AB-9E32-3CF5343B65C8}" name="Test Type"/>
+    <tableColumn id="7" xr3:uid="{D4902FDF-0C33-47F9-A7AD-166C2731D391}" name="NOTES"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Screenshots Worksheet Link" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1197,250 +1388,357 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="85.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.109375" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" customWidth="1"/>
     <col min="3" max="3" width="85.109375" customWidth="1"/>
-    <col min="4" max="5" width="35.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="28.44140625" customWidth="1"/>
-    <col min="11" max="11" width="12.21875" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" customWidth="1"/>
-    <col min="14" max="14" width="9.77734375" customWidth="1"/>
-    <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="28.44140625" customWidth="1"/>
+    <col min="4" max="6" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" customWidth="1"/>
+    <col min="15" max="15" width="9.77734375" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="63.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4"/>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <f>HYPERLINK("#Screenshots!A31", "Multi-Factor Authentication Screen")</f>
+        <v>Multi-Factor Authentication Screen</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="5" t="str">
+        <f>HYPERLINK("#Screenshots!A5", "Invalid username/password Screen")</f>
+        <v>Invalid username/password Screen</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="5" t="str">
+        <f>HYPERLINK("#Screenshots!A50", "Forgot your password? Screen")</f>
+        <v>Forgot your password? Screen</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <f>HYPERLINK("#Screenshots!A69", "Account Registration Screen")</f>
+        <v>Account Registration Screen</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="6" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="6" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="6" t="s">
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="6" t="s">
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="E17" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="E22" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter details in table below" sqref="A1:E1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading. Use heading filters to find specific entries" sqref="A2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Guest names in this column under this heading" sqref="B2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="E2:F2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter details in table below" sqref="A1:F1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Menu in this column under this heading" sqref="C2:D2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="E2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
@@ -1456,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B538E2A-57E0-451C-ABED-7DC529D936A2}">
   <dimension ref="A1:A182"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="A181" sqref="A181"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1467,45 +1765,45 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
+      <c r="A2" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
-        <v>20</v>
+      <c r="A108" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1519,86 +1817,376 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A26683-2EA6-4241-ABFD-DAC89CE652B7}">
-  <dimension ref="A1:A67"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="100.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>45</v>
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+    </row>
+    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="10"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="10"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="10"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+    </row>
+    <row r="53" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="10"/>
+      <c r="B53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="10"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="10"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="10"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="10"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="10"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="10"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="10"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="10"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="10"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="10"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="10"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="10"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="10"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="10"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="10"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="10"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="10"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="10"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="10"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="10"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="10"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="10"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="10"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="10"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="10"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="10"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="10"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="10"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="10"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="10"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="10"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="10"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="10"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="10"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="10"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="10"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="10"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="10"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="10"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="10"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="10"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="10"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="10"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="10"/>
+    </row>
+    <row r="102" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A102" s="10">
+        <v>4</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="10"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="10"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="10">
+        <v>5</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -1809,25 +2397,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1098FAC-3035-4AE0-8077-2547BF02CCCE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4B1929B-CBBD-4946-8F26-9E751F4BBB53}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{784530BF-A6E5-4879-8653-D651253C5B1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1844,4 +2431,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4B1929B-CBBD-4946-8F26-9E751F4BBB53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1098FAC-3035-4AE0-8077-2547BF02CCCE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>